<commit_message>
Update UART + schematic
</commit_message>
<xml_diff>
--- a/C3-27-epaper-touch/production/C3-27-BOM.xlsx
+++ b/C3-27-epaper-touch/production/C3-27-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
   <si>
     <t>C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>C1779</t>
-  </si>
-  <si>
-    <t>ESP32-C3-WROOM-02-N4</t>
   </si>
   <si>
     <t>SOT-23</t>
@@ -125,10 +122,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -203,125 +200,127 @@
     <row r="4" spans="1:4" ht="13.5">
       <c r="A4" t="inlineStr">
         <is>
-          <t>U1</t>
+          <t>Q2,Q3</t>
         </is>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>BC817</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C2934560</t>
+          <t>C146798</t>
         </is>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Q2,Q3</t>
+          <t>C8,C4,C6,C5</t>
         </is>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BC817</t>
+          <t>1uF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C146798</t>
+          <t>C28323</t>
         </is>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.5">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C8,C4,C6,C5</t>
-        </is>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
+          <t>J2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>USB_C_Receptacle_HRO_TYPE-C-31-M-12</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1uF</t>
+          <t>USB_C_Programming</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C28323</t>
+          <t>C165948</t>
         </is>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.5">
       <c r="A7" t="inlineStr">
         <is>
-          <t>J2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>USB_C_Receptacle_HRO_TYPE-C-31-M-12</t>
-        </is>
+          <t>U3</t>
+        </is>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>USB_C_Programming</t>
+          <t>MCP1700-3302E_SOT23</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C165948</t>
+          <t>C39051</t>
         </is>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.5">
       <c r="A8" t="inlineStr">
         <is>
-          <t>U3</t>
+          <t>C11</t>
         </is>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MCP1700-3302E_SOT23</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>C39051</t>
-        </is>
+          <t>4.7uF 50V</t>
+        </is>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.5">
       <c r="A9" t="inlineStr">
         <is>
-          <t>C11</t>
+          <t>R11</t>
         </is>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>4.7uF 50V</t>
-        </is>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
+          <t>0.47R</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>C103895</t>
+        </is>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.5">
       <c r="A10" t="inlineStr">
         <is>
-          <t>R11</t>
+          <t>C17,C18</t>
         </is>
       </c>
       <c r="B10" t="s">
@@ -329,221 +328,221 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.47R</t>
+          <t>220uF</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>C103895</t>
+          <t>C122252</t>
         </is>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.5">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C17,C18</t>
-        </is>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
+          <t>U4</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>220uF</t>
+          <t>DS3231MZ</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>C122252</t>
+          <t>C107410</t>
         </is>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.5">
       <c r="A12" t="inlineStr">
         <is>
-          <t>U4</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-        </is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DS3231MZ</t>
+          <t>3R</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>C107410</t>
+          <t>C25237</t>
         </is>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.5">
       <c r="A13" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R2,R5,R12,R4</t>
         </is>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3R</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C25237</t>
-        </is>
+          <t>10 K</t>
+        </is>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.5">
       <c r="A14" t="inlineStr">
         <is>
-          <t>R2,R5,R12,R4</t>
-        </is>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
+          <t>JP1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>switch-MK-12C02-G020</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10 K</t>
-        </is>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
+          <t>RESE</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>C2911519</t>
+        </is>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.5">
       <c r="A15" t="inlineStr">
         <is>
-          <t>JP1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>switch-MK-12C02-G020</t>
-        </is>
+          <t>C14,C15</t>
+        </is>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>RESE</t>
+          <t>10uF</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>C2911519</t>
+          <t>C15850</t>
         </is>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C14,C15</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>10uF</t>
-        </is>
+      <c r="C16" t="s">
+        <v>8</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>C15850</t>
+          <t>C262292</t>
         </is>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.5">
       <c r="A17" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>R7,R6</t>
         </is>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>5.1K</t>
+        </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>C262292</t>
+          <t>C23186</t>
         </is>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5">
       <c r="A18" t="inlineStr">
         <is>
-          <t>R7,R6</t>
-        </is>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
+          <t>D1,D3,D2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>D_SOD-123</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>5.1K</t>
+          <t>MBR0530</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>C23186</t>
+          <t>C77336</t>
         </is>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13.5">
       <c r="A19" t="inlineStr">
         <is>
-          <t>D1,D3,D2</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>D_SOD-123</t>
-        </is>
+          <t>C13</t>
+        </is>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MBR0530</t>
+          <t>100 nF</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>C77336</t>
+          <t>C28233</t>
         </is>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.5">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C13</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>100 nF</t>
+          <t>3.6K</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>C28233</t>
+          <t>C22980</t>
         </is>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.5">
       <c r="A21" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>C16</t>
         </is>
       </c>
       <c r="B21" t="s">
@@ -551,176 +550,156 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3.6K</t>
+          <t>C_Polarized 100uF</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>C22980</t>
+          <t>C129289</t>
         </is>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.5">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C16</t>
+          <t>R1</t>
         </is>
       </c>
       <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>10K</t>
+        </is>
+      </c>
+      <c r="D22" t="s">
         <v>6</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>C_Polarized 100uF</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>C129289</t>
-        </is>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.5">
       <c r="A23" t="inlineStr">
         <is>
-          <t>R1</t>
-        </is>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
+          <t>J4</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FH34SRJ-6S-0.5SH50-Hirose</t>
+        </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10K</t>
-        </is>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
+          <t>Conn_01x06_Female</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>C224194</t>
+        </is>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5">
       <c r="A24" t="inlineStr">
         <is>
-          <t>J4</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>FH34SRJ-6S-0.5SH50-Hirose</t>
-        </is>
+          <t>R9,R8</t>
+        </is>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Conn_01x06_Female</t>
+          <t>4.7K</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>C224194</t>
+          <t>C23162</t>
         </is>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.5">
       <c r="A25" t="inlineStr">
         <is>
-          <t>R9,R8</t>
-        </is>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
+          <t>U2</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>QFN-24-1EP_4x4mm_P0.5mm_EP2.6x2.6mm</t>
+        </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4.7K</t>
+          <t>CP2102N-Axx-xQFN24</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>C23162</t>
+          <t>C964632</t>
         </is>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5">
       <c r="A26" t="inlineStr">
         <is>
-          <t>U2</t>
+          <t>Q1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>QFN-24-1EP_4x4mm_P0.5mm_EP2.6x2.6mm</t>
+          <t>SOT-323_SC-70</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CP2102N-Axx-xQFN24</t>
+          <t>Si1308</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>C964632</t>
+          <t>C469327</t>
         </is>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.5">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>C12</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SOT-323_SC-70</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Si1308</t>
-        </is>
+          <t>C_0603_1608Metric</t>
+        </is>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>C469327</t>
+          <t>C19666</t>
         </is>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.5">
       <c r="A28" t="inlineStr">
         <is>
-          <t>C12</t>
+          <t>L1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>C_0603_1608Metric</t>
-        </is>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
+          <t>SWPA4030S1R0NT</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>10uH</t>
+        </is>
       </c>
       <c r="D28" t="inlineStr">
-        <is>
-          <t>C19666</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="13.5">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>SWPA4030S1R0NT</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>10uH</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
         <is>
           <t>C38117</t>
         </is>

</xml_diff>

<commit_message>
Update C3 with new CP2102 according to spec
</commit_message>
<xml_diff>
--- a/C3-27-epaper-touch/production/C3-27-BOM.xlsx
+++ b/C3-27-epaper-touch/production/C3-27-BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="9890" windowHeight="8060"/>
+    <workbookView activeTab="0" windowWidth="14400" windowHeight="6020"/>
   </bookViews>
   <sheets>
     <sheet name="C3-27-epaper-touch.csv" sheetId="1" r:id="rId1"/>
@@ -122,10 +122,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0" tabSelected="1">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -184,7 +184,7 @@
     <row r="3" spans="1:4" ht="13.5">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C2,C7,C9,C10,C1,C3</t>
+          <t>C2,C7,C9,C10,C19,C1,C3</t>
         </is>
       </c>
       <c r="B3" t="s">
@@ -282,107 +282,107 @@
     <row r="8" spans="1:4" ht="13.5">
       <c r="A8" t="inlineStr">
         <is>
-          <t>C11</t>
+          <t>R13</t>
         </is>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>4.7uF 50V</t>
-        </is>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
+          <t>1K</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>C21190</t>
+        </is>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.5">
       <c r="A9" t="inlineStr">
         <is>
-          <t>R11</t>
+          <t>C11</t>
         </is>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.47R</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>C103895</t>
-        </is>
+          <t>4.7uF 50V</t>
+        </is>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.5">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C17,C18</t>
+          <t>R11</t>
         </is>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>220uF</t>
+          <t>0.47R</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>C122252</t>
+          <t>C103895</t>
         </is>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.5">
       <c r="A11" t="inlineStr">
         <is>
-          <t>U4</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-        </is>
+          <t>C17,C18</t>
+        </is>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DS3231MZ</t>
+          <t>220uF</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>C107410</t>
+          <t>C122252</t>
         </is>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.5">
       <c r="A12" t="inlineStr">
         <is>
-          <t>R3</t>
-        </is>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
+          <t>U4</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3R</t>
+          <t>DS3231MZ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>C25237</t>
+          <t>C107410</t>
         </is>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.5">
       <c r="A13" t="inlineStr">
         <is>
-          <t>R2,R5,R12,R4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="B13" t="s">
@@ -390,318 +390,382 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10 K</t>
-        </is>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
+          <t>3R</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C25237</t>
+        </is>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.5">
       <c r="A14" t="inlineStr">
         <is>
-          <t>JP1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>switch-MK-12C02-G020</t>
-        </is>
+          <t>R2,R5,R12,R4</t>
+        </is>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RESE</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>C2911519</t>
-        </is>
+          <t>10 K</t>
+        </is>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.5">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C14,C15</t>
-        </is>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
+          <t>JP1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>switch-MK-12C02-G020</t>
+        </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>10uF</t>
+          <t>RESE</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>C15850</t>
+          <t>C2911519</t>
         </is>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5">
       <c r="A16" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>C14,C15</t>
         </is>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>10uF</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>C262292</t>
+          <t>C15850</t>
         </is>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.5">
       <c r="A17" t="inlineStr">
         <is>
-          <t>R7,R6</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>5.1K</t>
-        </is>
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>C23186</t>
+          <t>C262292</t>
         </is>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5">
       <c r="A18" t="inlineStr">
         <is>
-          <t>D1,D3,D2</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>D_SOD-123</t>
-        </is>
+          <t>R7,R6</t>
+        </is>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MBR0530</t>
+          <t>5.1K</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>C77336</t>
+          <t>C23186</t>
         </is>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13.5">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C13</t>
-        </is>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
+          <t>D1,D3,D2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>D_SOD-123</t>
+        </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>100 nF</t>
+          <t>MBR0530</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>C28233</t>
+          <t>C77336</t>
         </is>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.5">
       <c r="A20" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>C13</t>
         </is>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3.6K</t>
+          <t>100nF</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>C22980</t>
+          <t>C28233</t>
         </is>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.5">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C16</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>C_Polarized 100uF</t>
+          <t>3.6K</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>C129289</t>
+          <t>C22980</t>
         </is>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.5">
       <c r="A22" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>C16</t>
         </is>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10K</t>
-        </is>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
+          <t>C_Polarized 100uF</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>C129289</t>
+        </is>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.5">
       <c r="A23" t="inlineStr">
         <is>
-          <t>J4</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>FH34SRJ-6S-0.5SH50-Hirose</t>
-        </is>
+          <t>R1</t>
+        </is>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Conn_01x06_Female</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>C224194</t>
-        </is>
+          <t>10K</t>
+        </is>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5">
       <c r="A24" t="inlineStr">
         <is>
-          <t>R9,R8</t>
-        </is>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
+          <t>J4</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>FH34SRJ-6S-0.5SH50-Hirose</t>
+        </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>4.7K</t>
+          <t>Conn_01x06_Female</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>C23162</t>
+          <t>C224194</t>
         </is>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.5">
       <c r="A25" t="inlineStr">
         <is>
-          <t>U2</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>QFN-24-1EP_4x4mm_P0.5mm_EP2.6x2.6mm</t>
-        </is>
+          <t>R9,R8</t>
+        </is>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CP2102N-Axx-xQFN24</t>
+          <t>4.7K</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>C964632</t>
+          <t>C23162</t>
         </is>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>U2</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SOT-323_SC-70</t>
+          <t>CP2102-QFN50P500X500X80-29N-D</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Si1308</t>
+          <t>CP2102N-A02-GQFN28R</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>C469327</t>
+          <t>C964632</t>
         </is>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.5">
       <c r="A27" t="inlineStr">
         <is>
-          <t>C12</t>
+          <t>R15</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>C_0603_1608Metric</t>
-        </is>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
+          <t>R_0402_1005Metric</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>47K</t>
+        </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>C19666</t>
+          <t>C137974</t>
         </is>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.5">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>SOT-323_SC-70</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Si1308</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>C469327</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="13.5">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C12</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>C_0603_1608Metric</t>
+        </is>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>C19666</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="13.5">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>L1</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>SWPA4030S1R0NT</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>10uH</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>C38117</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="13.5">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>R14</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>R_0201_0603Metric</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>22K</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>C31850</t>
         </is>
       </c>
     </row>

</xml_diff>